<commit_message>
drop down stat-list added
</commit_message>
<xml_diff>
--- a/app/mediafiles/out.xlsx
+++ b/app/mediafiles/out.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="43">
   <si>
     <t>Вопрос</t>
   </si>
@@ -58,13 +58,13 @@
     <t>Губкинское ЛПУМГ (КС - 03, Общежитие №1)</t>
   </si>
   <si>
+    <t>Н-Уренгойское ЛПУМГ (ПВП № 1, КС Пуртазовская)</t>
+  </si>
+  <si>
     <t>Название_ПВИ</t>
   </si>
   <si>
     <t>Местонахождение_ПВИ</t>
-  </si>
-  <si>
-    <t>Н-Уренгойское ЛПУМГ (ПВП № 1, КС Пуртазовская)</t>
   </si>
   <si>
     <t>Н-Уренгойское ЛПУМГ (ПВП №2)</t>
@@ -561,7 +561,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -792,6 +792,75 @@
       </c>
       <c r="G10" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>99295</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="2">
+        <v>44165</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>99295</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="2">
+        <v>44165</v>
+      </c>
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>99295</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="2">
+        <v>44165</v>
+      </c>
+      <c r="G13" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -809,10 +878,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -820,7 +889,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
added drop down stats
</commit_message>
<xml_diff>
--- a/app/mediafiles/out.xlsx
+++ b/app/mediafiles/out.xlsx
@@ -17,7 +17,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="43">
+  <si>
+    <t>Номер_Вопроса</t>
+  </si>
   <si>
     <t>Вопрос</t>
   </si>
@@ -52,25 +55,22 @@
     <t>None</t>
   </si>
   <si>
-    <t>Н-Уренгойское ЛПУМГ (КС Пуртазовская)</t>
+    <t>Н-Уренгойское ЛПУМГ (ПВП № 1, КС Пуртазовская)</t>
+  </si>
+  <si>
+    <t>Н-Уренгойское ЛПУМГ (ПВП №2)</t>
+  </si>
+  <si>
+    <t>Пурпейское ЛПУМГ (КС - 01, Общежитие на 100 мест Ягенетская п/п)</t>
+  </si>
+  <si>
+    <t>Название_ПВИ</t>
+  </si>
+  <si>
+    <t>Местонахождение_ПВИ</t>
   </si>
   <si>
     <t>Губкинское ЛПУМГ (КС - 03, Общежитие №1)</t>
-  </si>
-  <si>
-    <t>Н-Уренгойское ЛПУМГ (ПВП № 1, КС Пуртазовская)</t>
-  </si>
-  <si>
-    <t>Название_ПВИ</t>
-  </si>
-  <si>
-    <t>Местонахождение_ПВИ</t>
-  </si>
-  <si>
-    <t>Н-Уренгойское ЛПУМГ (ПВП №2)</t>
-  </si>
-  <si>
-    <t>Пурпейское ЛПУМГ (КС - 01, Общежитие на 100 мест Ягенетская п/п)</t>
   </si>
   <si>
     <t>Демьянское ЛПУМГ (КС - 7, Общежитие в п. Демьянка)</t>
@@ -507,50 +507,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2">
+        <v>44161</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2">
         <v>44161</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2">
-        <v>44161</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2">
         <v>44161</v>
       </c>
     </row>
@@ -569,22 +581,22 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -592,22 +604,22 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>186933</v>
+        <v>179182</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="2">
         <v>44165</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -615,22 +627,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>186933</v>
+        <v>179182</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" s="2">
         <v>44165</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -638,22 +650,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>186933</v>
+        <v>179182</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" s="2">
         <v>44165</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -661,22 +673,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>217166</v>
+        <v>212300</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F5" s="2">
         <v>44165</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -684,22 +696,22 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>217166</v>
+        <v>212300</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F6" s="2">
         <v>44165</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -707,22 +719,22 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>217166</v>
+        <v>212300</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F7" s="2">
         <v>44165</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -730,22 +742,22 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>136953</v>
+        <v>13679</v>
       </c>
       <c r="C8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F8" s="2">
         <v>44165</v>
       </c>
       <c r="G8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -753,22 +765,22 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>136953</v>
+        <v>13679</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F9" s="2">
         <v>44165</v>
       </c>
       <c r="G9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -776,22 +788,22 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>136953</v>
+        <v>13679</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F10" s="2">
         <v>44165</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -799,22 +811,22 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>99295</v>
+        <v>146533</v>
       </c>
       <c r="C11" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F11" s="2">
         <v>44165</v>
       </c>
       <c r="G11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -822,22 +834,22 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>99295</v>
+        <v>146533</v>
       </c>
       <c r="C12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F12" s="2">
         <v>44165</v>
       </c>
       <c r="G12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -845,22 +857,22 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>99295</v>
+        <v>146533</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F13" s="2">
         <v>44165</v>
       </c>
       <c r="G13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -878,10 +890,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -889,7 +901,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
         <v>27</v>
@@ -900,7 +912,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
@@ -911,7 +923,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>29</v>
@@ -922,7 +934,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
         <v>30</v>
@@ -1042,7 +1054,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Added filters to admin page
</commit_message>
<xml_diff>
--- a/app/mediafiles/out.xlsx
+++ b/app/mediafiles/out.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="41">
   <si>
     <t>Номер_Вопроса</t>
   </si>
@@ -28,13 +28,13 @@
     <t>Дата создания</t>
   </si>
   <si>
-    <t>Довольны ли Вы качеством предоставляемого питания?</t>
-  </si>
-  <si>
-    <t>Устраивают ли Вас бытовые условия? (питьевой режим, температура в помещении, досуг и психологический климат)</t>
-  </si>
-  <si>
-    <t>Довольны ли Вы работой обслуживающего персонала?</t>
+    <t>Первый вопрос</t>
+  </si>
+  <si>
+    <t>Второй вопрос</t>
+  </si>
+  <si>
+    <t>Третий вопрос</t>
   </si>
   <si>
     <t>unique_key</t>
@@ -64,6 +64,12 @@
     <t>Пурпейское ЛПУМГ (КС - 01, Общежитие на 100 мест Ягенетская п/п)</t>
   </si>
   <si>
+    <t>Демьянское ЛПУМГ (КС - 7, Общежитие в п. Демьянка)</t>
+  </si>
+  <si>
+    <t>Сургутское ЛПУМГ (УСС "Факел")</t>
+  </si>
+  <si>
     <t>Название_ПВИ</t>
   </si>
   <si>
@@ -73,9 +79,6 @@
     <t>Губкинское ЛПУМГ (КС - 03, Общежитие №1)</t>
   </si>
   <si>
-    <t>Демьянское ЛПУМГ (КС - 7, Общежитие в п. Демьянка)</t>
-  </si>
-  <si>
     <t>Туртасское ЛПУМГ (КС-8, Общежитие в п. Пионерный)</t>
   </si>
   <si>
@@ -85,9 +88,6 @@
     <t>Вынгапуровское ЛПУМГ (КС-1, Общежитие)</t>
   </si>
   <si>
-    <t>Сургутское ЛПУМГ (УСС "Факел")</t>
-  </si>
-  <si>
     <t>Сургутское ЛПУМГ (КС-3, Общежитие)</t>
   </si>
   <si>
@@ -140,12 +140,6 @@
   </si>
   <si>
     <t>Пожелание</t>
-  </si>
-  <si>
-    <t>Очень положительный комент</t>
-  </si>
-  <si>
-    <t>Общий комментарий</t>
   </si>
 </sst>
 </file>
@@ -535,7 +529,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="2">
-        <v>44161</v>
+        <v>44165</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -549,7 +543,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="2">
-        <v>44161</v>
+        <v>44165</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -563,7 +557,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="2">
-        <v>44161</v>
+        <v>44165</v>
       </c>
     </row>
   </sheetData>
@@ -573,7 +567,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -604,7 +598,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>179182</v>
+        <v>78035</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -627,7 +621,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>179182</v>
+        <v>78035</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -650,7 +644,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>179182</v>
+        <v>78035</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -673,7 +667,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>212300</v>
+        <v>142820</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
@@ -688,7 +682,7 @@
         <v>44165</v>
       </c>
       <c r="G5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -696,7 +690,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>212300</v>
+        <v>142820</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -711,7 +705,7 @@
         <v>44165</v>
       </c>
       <c r="G6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -719,7 +713,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>212300</v>
+        <v>142820</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -734,7 +728,7 @@
         <v>44165</v>
       </c>
       <c r="G7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -742,7 +736,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>13679</v>
+        <v>150831</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
@@ -757,7 +751,7 @@
         <v>44165</v>
       </c>
       <c r="G8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -765,7 +759,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>13679</v>
+        <v>150831</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -780,7 +774,7 @@
         <v>44165</v>
       </c>
       <c r="G9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -788,7 +782,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>13679</v>
+        <v>150831</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -803,7 +797,7 @@
         <v>44165</v>
       </c>
       <c r="G10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -811,7 +805,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>146533</v>
+        <v>9022</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
@@ -826,7 +820,7 @@
         <v>44165</v>
       </c>
       <c r="G11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -834,7 +828,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>146533</v>
+        <v>9022</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -849,7 +843,7 @@
         <v>44165</v>
       </c>
       <c r="G12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -857,7 +851,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>146533</v>
+        <v>9022</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -872,6 +866,558 @@
         <v>44165</v>
       </c>
       <c r="G13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>218044</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="2">
+        <v>44165</v>
+      </c>
+      <c r="G14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>218044</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="2">
+        <v>44165</v>
+      </c>
+      <c r="G15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>218044</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="2">
+        <v>44165</v>
+      </c>
+      <c r="G16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>233672</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="2">
+        <v>44165</v>
+      </c>
+      <c r="G17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>233672</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="2">
+        <v>44165</v>
+      </c>
+      <c r="G18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>233672</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="2">
+        <v>44165</v>
+      </c>
+      <c r="G19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>265177</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="2">
+        <v>44165</v>
+      </c>
+      <c r="G20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>265177</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="2">
+        <v>44165</v>
+      </c>
+      <c r="G21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>265177</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="2">
+        <v>44165</v>
+      </c>
+      <c r="G22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>292964</v>
+      </c>
+      <c r="C23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="2">
+        <v>44167</v>
+      </c>
+      <c r="G23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>292964</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="2">
+        <v>44167</v>
+      </c>
+      <c r="G24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>292964</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="2">
+        <v>44167</v>
+      </c>
+      <c r="G25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>137897</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="2">
+        <v>44167</v>
+      </c>
+      <c r="G26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>137897</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="2">
+        <v>44167</v>
+      </c>
+      <c r="G27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>137897</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
+      <c r="E28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="2">
+        <v>44167</v>
+      </c>
+      <c r="G28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>177809</v>
+      </c>
+      <c r="C29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29">
+        <v>3</v>
+      </c>
+      <c r="E29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="2">
+        <v>44167</v>
+      </c>
+      <c r="G29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>177809</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30">
+        <v>3</v>
+      </c>
+      <c r="E30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="2">
+        <v>44167</v>
+      </c>
+      <c r="G30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>177809</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="E31" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="2">
+        <v>44167</v>
+      </c>
+      <c r="G31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>238761</v>
+      </c>
+      <c r="C32" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32">
+        <v>5</v>
+      </c>
+      <c r="E32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="2">
+        <v>44167</v>
+      </c>
+      <c r="G32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>238761</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33">
+        <v>5</v>
+      </c>
+      <c r="E33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="2">
+        <v>44167</v>
+      </c>
+      <c r="G33" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>238761</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
+      </c>
+      <c r="E34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="2">
+        <v>44167</v>
+      </c>
+      <c r="G34" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>198786</v>
+      </c>
+      <c r="C35" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35">
+        <v>5</v>
+      </c>
+      <c r="E35" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" s="2">
+        <v>44167</v>
+      </c>
+      <c r="G35" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>198786</v>
+      </c>
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>5</v>
+      </c>
+      <c r="E36" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="2">
+        <v>44167</v>
+      </c>
+      <c r="G36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>198786</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37">
+        <v>3</v>
+      </c>
+      <c r="E37" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" s="2">
+        <v>44167</v>
+      </c>
+      <c r="G37" t="s">
         <v>12</v>
       </c>
     </row>
@@ -890,10 +1436,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -934,7 +1480,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
         <v>30</v>
@@ -945,7 +1491,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
         <v>31</v>
@@ -956,7 +1502,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
         <v>32</v>
@@ -967,7 +1513,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
         <v>33</v>
@@ -978,7 +1524,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
         <v>34</v>
@@ -989,7 +1535,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
         <v>35</v>
@@ -1046,40 +1592,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="B1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="2:3">
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>24057</v>
-      </c>
-      <c r="C2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>233336</v>
-      </c>
-      <c r="C3" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
separate admin and users stats
</commit_message>
<xml_diff>
--- a/app/mediafiles/out.xlsx
+++ b/app/mediafiles/out.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1845" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1854" uniqueCount="198">
   <si>
     <t>Номер_Вопроса</t>
   </si>
@@ -429,6 +429,9 @@
   </si>
   <si>
     <t>Сургутское ЛПУМГ (УСС "Факел")</t>
+  </si>
+  <si>
+    <t>(КС-2) Ортьягунское ЛПУМГ</t>
   </si>
   <si>
     <t>Название_ПВИ</t>
@@ -1053,7 +1056,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G586"/>
+  <dimension ref="A1:G589"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -14532,6 +14535,75 @@
       </c>
       <c r="G586" t="s">
         <v>133</v>
+      </c>
+    </row>
+    <row r="587" spans="1:7">
+      <c r="A587" s="1">
+        <v>585</v>
+      </c>
+      <c r="B587">
+        <v>57434</v>
+      </c>
+      <c r="C587" t="s">
+        <v>3</v>
+      </c>
+      <c r="D587">
+        <v>5</v>
+      </c>
+      <c r="E587" t="s">
+        <v>11</v>
+      </c>
+      <c r="F587" s="2">
+        <v>44178</v>
+      </c>
+      <c r="G587" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="588" spans="1:7">
+      <c r="A588" s="1">
+        <v>586</v>
+      </c>
+      <c r="B588">
+        <v>57434</v>
+      </c>
+      <c r="C588" t="s">
+        <v>4</v>
+      </c>
+      <c r="D588">
+        <v>5</v>
+      </c>
+      <c r="E588" t="s">
+        <v>11</v>
+      </c>
+      <c r="F588" s="2">
+        <v>44178</v>
+      </c>
+      <c r="G588" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="589" spans="1:7">
+      <c r="A589" s="1">
+        <v>587</v>
+      </c>
+      <c r="B589">
+        <v>57434</v>
+      </c>
+      <c r="C589" t="s">
+        <v>5</v>
+      </c>
+      <c r="D589">
+        <v>5</v>
+      </c>
+      <c r="E589" t="s">
+        <v>11</v>
+      </c>
+      <c r="F589" s="2">
+        <v>44178</v>
+      </c>
+      <c r="G589" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -14549,10 +14621,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="B1" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -14563,7 +14635,7 @@
         <v>125</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -14571,10 +14643,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -14585,7 +14657,7 @@
         <v>126</v>
       </c>
       <c r="C4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -14596,7 +14668,7 @@
         <v>124</v>
       </c>
       <c r="C5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -14604,10 +14676,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -14618,7 +14690,7 @@
         <v>123</v>
       </c>
       <c r="C7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -14629,7 +14701,7 @@
         <v>132</v>
       </c>
       <c r="C8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -14640,7 +14712,7 @@
         <v>128</v>
       </c>
       <c r="C9" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -14651,7 +14723,7 @@
         <v>133</v>
       </c>
       <c r="C10" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -14662,7 +14734,7 @@
         <v>127</v>
       </c>
       <c r="C11" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -14673,7 +14745,7 @@
         <v>130</v>
       </c>
       <c r="C12" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -14684,7 +14756,7 @@
         <v>131</v>
       </c>
       <c r="C13" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -14692,10 +14764,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="C14" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -14716,7 +14788,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -14727,7 +14799,7 @@
         <v>24057</v>
       </c>
       <c r="C2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -14738,7 +14810,7 @@
         <v>233336</v>
       </c>
       <c r="C3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -14749,7 +14821,7 @@
         <v>258094</v>
       </c>
       <c r="C4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -14760,7 +14832,7 @@
         <v>107781</v>
       </c>
       <c r="C5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -14771,7 +14843,7 @@
         <v>216148</v>
       </c>
       <c r="C6" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -14782,7 +14854,7 @@
         <v>214558</v>
       </c>
       <c r="C7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -14793,7 +14865,7 @@
         <v>5871</v>
       </c>
       <c r="C8" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -14804,7 +14876,7 @@
         <v>80327</v>
       </c>
       <c r="C9" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -14815,7 +14887,7 @@
         <v>232342</v>
       </c>
       <c r="C10" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -14826,7 +14898,7 @@
         <v>215485</v>
       </c>
       <c r="C11" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -14837,7 +14909,7 @@
         <v>106616</v>
       </c>
       <c r="C12" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -14848,7 +14920,7 @@
         <v>293274</v>
       </c>
       <c r="C13" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -14859,7 +14931,7 @@
         <v>137281</v>
       </c>
       <c r="C14" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -14870,7 +14942,7 @@
         <v>215431</v>
       </c>
       <c r="C15" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -14881,7 +14953,7 @@
         <v>208016</v>
       </c>
       <c r="C16" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -14892,7 +14964,7 @@
         <v>227785</v>
       </c>
       <c r="C17" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -14903,7 +14975,7 @@
         <v>107364</v>
       </c>
       <c r="C18" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -14914,7 +14986,7 @@
         <v>284926</v>
       </c>
       <c r="C19" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -14925,7 +14997,7 @@
         <v>124609</v>
       </c>
       <c r="C20" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -14936,7 +15008,7 @@
         <v>183271</v>
       </c>
       <c r="C21" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -14947,7 +15019,7 @@
         <v>214182</v>
       </c>
       <c r="C22" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -14958,7 +15030,7 @@
         <v>126371</v>
       </c>
       <c r="C23" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -14969,7 +15041,7 @@
         <v>218071</v>
       </c>
       <c r="C24" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -14980,7 +15052,7 @@
         <v>277513</v>
       </c>
       <c r="C25" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -14991,7 +15063,7 @@
         <v>112959</v>
       </c>
       <c r="C26" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -15002,7 +15074,7 @@
         <v>278974</v>
       </c>
       <c r="C27" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -15013,7 +15085,7 @@
         <v>50154</v>
       </c>
       <c r="C28" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -15024,7 +15096,7 @@
         <v>258548</v>
       </c>
       <c r="C29" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -15035,7 +15107,7 @@
         <v>48868</v>
       </c>
       <c r="C30" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -15046,7 +15118,7 @@
         <v>239683</v>
       </c>
       <c r="C31" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -15057,7 +15129,7 @@
         <v>42165</v>
       </c>
       <c r="C32" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -15068,7 +15140,7 @@
         <v>218901</v>
       </c>
       <c r="C33" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -15079,7 +15151,7 @@
         <v>166374</v>
       </c>
       <c r="C34" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -15090,7 +15162,7 @@
         <v>231747</v>
       </c>
       <c r="C35" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -15101,7 +15173,7 @@
         <v>31016</v>
       </c>
       <c r="C36" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -15112,7 +15184,7 @@
         <v>21933</v>
       </c>
       <c r="C37" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -15123,7 +15195,7 @@
         <v>152440</v>
       </c>
       <c r="C38" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -15134,7 +15206,7 @@
         <v>217149</v>
       </c>
       <c r="C39" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -15145,7 +15217,7 @@
         <v>58273</v>
       </c>
       <c r="C40" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -15156,7 +15228,7 @@
         <v>153489</v>
       </c>
       <c r="C41" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -15167,7 +15239,7 @@
         <v>297019</v>
       </c>
       <c r="C42" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -15178,7 +15250,7 @@
         <v>267752</v>
       </c>
       <c r="C43" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -15189,7 +15261,7 @@
         <v>219521</v>
       </c>
       <c r="C44" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -15200,7 +15272,7 @@
         <v>229749</v>
       </c>
       <c r="C45" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -15211,7 +15283,7 @@
         <v>119098</v>
       </c>
       <c r="C46" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -15222,7 +15294,7 @@
         <v>284142</v>
       </c>
       <c r="C47" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -15233,7 +15305,7 @@
         <v>205192</v>
       </c>
       <c r="C48" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -15244,7 +15316,7 @@
         <v>126808</v>
       </c>
       <c r="C49" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>